<commit_message>
Penambahan Trello dan BurndownChart
</commit_message>
<xml_diff>
--- a/BurndownChartProjectTKPPL.xlsx
+++ b/BurndownChartProjectTKPPL.xlsx
@@ -10,7 +10,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -109,14 +108,6 @@
     </font>
     <font>
       <b/>
-      <sz val="14"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -127,6 +118,13 @@
       <b/>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -165,7 +163,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -250,15 +248,15 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -273,9 +271,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -287,6 +282,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -332,7 +330,7 @@
           <c:yMode val="edge"/>
           <c:x val="5.0233909198422112E-2"/>
           <c:y val="0.17487878043058086"/>
-          <c:w val="0.93419443723018569"/>
+          <c:w val="0.93419443723018591"/>
           <c:h val="0.80708212765482035"/>
         </c:manualLayout>
       </c:layout>
@@ -592,24 +590,24 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="62379136"/>
-        <c:axId val="62380672"/>
+        <c:axId val="56297344"/>
+        <c:axId val="56298880"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="62379136"/>
+        <c:axId val="56297344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62380672"/>
+        <c:crossAx val="56298880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="62380672"/>
+        <c:axId val="56298880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -617,7 +615,7 @@
         <c:minorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62379136"/>
+        <c:crossAx val="56297344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -630,7 +628,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -926,7 +924,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -937,7 +935,7 @@
   <dimension ref="A1:S71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="M47" sqref="M47"/>
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -955,22 +953,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="27.75" customHeight="1">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
     </row>
     <row r="2" spans="1:19" ht="27.75" customHeight="1"/>
     <row r="3" spans="1:19" ht="27.75" customHeight="1"/>
@@ -1037,7 +1035,7 @@
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -1094,7 +1092,7 @@
     </row>
     <row r="6" spans="1:19" ht="27.75" customHeight="1">
       <c r="A6" s="3"/>
-      <c r="B6" s="13"/>
+      <c r="B6" s="12"/>
       <c r="C6" s="3" t="s">
         <v>9</v>
       </c>
@@ -1149,7 +1147,7 @@
     </row>
     <row r="7" spans="1:19" ht="27.75" customHeight="1">
       <c r="A7" s="3"/>
-      <c r="B7" s="14"/>
+      <c r="B7" s="13"/>
       <c r="C7" s="3"/>
       <c r="D7" s="8">
         <v>0</v>
@@ -1233,7 +1231,7 @@
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -1290,7 +1288,7 @@
     </row>
     <row r="10" spans="1:19" ht="27.75" customHeight="1">
       <c r="A10" s="3"/>
-      <c r="B10" s="13"/>
+      <c r="B10" s="12"/>
       <c r="C10" s="3" t="s">
         <v>12</v>
       </c>
@@ -1345,7 +1343,7 @@
     </row>
     <row r="11" spans="1:19" ht="27.75" customHeight="1">
       <c r="A11" s="3"/>
-      <c r="B11" s="14"/>
+      <c r="B11" s="13"/>
       <c r="C11" s="3" t="s">
         <v>13</v>
       </c>
@@ -1423,7 +1421,7 @@
       <c r="A13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1480,7 +1478,7 @@
     </row>
     <row r="14" spans="1:19" ht="27.75" customHeight="1">
       <c r="A14" s="3"/>
-      <c r="B14" s="13"/>
+      <c r="B14" s="12"/>
       <c r="C14" s="3" t="s">
         <v>16</v>
       </c>
@@ -1535,7 +1533,7 @@
     </row>
     <row r="15" spans="1:19" ht="27.75" customHeight="1">
       <c r="A15" s="3"/>
-      <c r="B15" s="14"/>
+      <c r="B15" s="13"/>
       <c r="C15" s="3" t="s">
         <v>17</v>
       </c>

</xml_diff>